<commit_message>
Added R1 and R2 to pindate
</commit_message>
<xml_diff>
--- a/Pin data.xlsx
+++ b/Pin data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Group-G-BattleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{256CFE8C-8D3C-40D1-AF2B-1A812F4420FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6039A82-4BAA-4C52-8458-AC3651F00581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="35" uniqueCount="33">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="38" uniqueCount="36">
   <si>
     <t>line sensor</t>
   </si>
@@ -124,13 +124,22 @@
   </si>
   <si>
     <t>Neo</t>
+  </si>
+  <si>
+    <t>R, aka the rotary sensors</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -143,8 +152,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +178,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,10 +197,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -493,11 +515,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,48 +630,69 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-  <pageSetup paperSize="0" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made the pulse sensor work. added bluetooth pins to the pindata file Made robot able to distinguish between an intersection and the end with pulse sensor
</commit_message>
<xml_diff>
--- a/Pin data.xlsx
+++ b/Pin data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Group-G-BattleBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E6039A82-4BAA-4C52-8458-AC3651F00581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{705A7648-1871-4852-B30B-FDD7B54EB287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="38" uniqueCount="36">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="43" uniqueCount="41">
   <si>
     <t>line sensor</t>
   </si>
@@ -133,6 +133,21 @@
   </si>
   <si>
     <t>R2</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>0RX</t>
+  </si>
+  <si>
+    <t>1TX</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HT</t>
   </si>
 </sst>
 </file>
@@ -159,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -184,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -197,11 +218,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -516,7 +538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -648,7 +670,7 @@
         <v>35</v>
       </c>
       <c r="B20">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -689,6 +711,27 @@
       </c>
       <c r="B26" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>